<commit_message>
se agregan escenarios de loguien exitosos
</commit_message>
<xml_diff>
--- a/build/resources/test/datadriven/login/testData.xlsx
+++ b/build/resources/test/datadriven/login/testData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\escritorio\bcs-loans-qa\src\test\resources\datadriven\login\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bcs-digital-credito\src\test\resources\datadriven\login\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C289B52-C16A-4652-9118-E3B71D2C09D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5BA952C-A9A4-48BF-B387-FAA66CAFCA70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9720" yWindow="345" windowWidth="24405" windowHeight="15585" activeTab="1" xr2:uid="{565A5E9C-6FFF-4ECB-8A93-B318EC1ABE36}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="5" xr2:uid="{565A5E9C-6FFF-4ECB-8A93-B318EC1ABE36}"/>
   </bookViews>
   <sheets>
     <sheet name="landing" sheetId="6" r:id="rId1"/>
@@ -18,11 +18,12 @@
     <sheet name="noChannels" sheetId="10" r:id="rId3"/>
     <sheet name="SuccessfulLogin" sheetId="11" r:id="rId4"/>
     <sheet name="ValidationDocumentNumber" sheetId="12" r:id="rId5"/>
-    <sheet name="happyPathCedula" sheetId="4" r:id="rId6"/>
-    <sheet name="loginValidationsButtonDisabled" sheetId="5" r:id="rId7"/>
-    <sheet name="loginValidationsmessage" sheetId="7" r:id="rId8"/>
-    <sheet name="Hoja1" sheetId="8" r:id="rId9"/>
-    <sheet name="loginValidations" sheetId="2" r:id="rId10"/>
+    <sheet name="validateModal" sheetId="13" r:id="rId6"/>
+    <sheet name="happyPathCedula" sheetId="4" r:id="rId7"/>
+    <sheet name="loginValidationsButtonDisabled" sheetId="5" r:id="rId8"/>
+    <sheet name="loginValidationsmessage" sheetId="7" r:id="rId9"/>
+    <sheet name="Hoja1" sheetId="8" r:id="rId10"/>
+    <sheet name="loginValidations" sheetId="2" r:id="rId11"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="89">
   <si>
     <t>idType</t>
   </si>
@@ -277,9 +278,6 @@
     <t>Bienvenido a</t>
   </si>
   <si>
-    <t>Monto</t>
-  </si>
-  <si>
     <t>Por su seguridad</t>
   </si>
   <si>
@@ -296,6 +294,21 @@
   </si>
   <si>
     <t>mauricio23456$</t>
+  </si>
+  <si>
+    <t>validando</t>
+  </si>
+  <si>
+    <t>loader</t>
+  </si>
+  <si>
+    <t>modal</t>
+  </si>
+  <si>
+    <t>Por favor verifique e intente de nuevo</t>
+  </si>
+  <si>
+    <t>Usuario bloqueado, por favor intente de nuevo en 24 horas</t>
   </si>
 </sst>
 </file>
@@ -684,6 +697,169 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A722FA9C-9A5F-4297-AFA4-6881D5BABD53}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1039458363</v>
+      </c>
+      <c r="E5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1039458363</v>
+      </c>
+      <c r="E6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49FBCBD8-D281-4F8A-96DE-EFE66D8A048C}">
   <dimension ref="A1:D19"/>
   <sheetViews>
@@ -972,8 +1148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{252687B5-B7E8-43A1-A660-258C89852C6D}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1016,7 +1192,7 @@
         <v>41728985</v>
       </c>
       <c r="E2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1055,7 +1231,7 @@
         <v>47</v>
       </c>
       <c r="E1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1072,7 +1248,7 @@
         <v>1030618791</v>
       </c>
       <c r="E2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1082,10 +1258,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{057BC5C0-1FAF-4790-BFEB-9F9EC877998A}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1095,10 +1271,11 @@
     <col min="3" max="3" width="20.85546875" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" customWidth="1"/>
-    <col min="7" max="7" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -1118,10 +1295,13 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>76</v>
       </c>
@@ -1132,19 +1312,22 @@
         <v>1</v>
       </c>
       <c r="D2" s="1">
-        <v>1026265690</v>
+        <v>10009287</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F2" t="s">
         <v>72</v>
       </c>
       <c r="G2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>76</v>
       </c>
@@ -1158,13 +1341,16 @@
         <v>1026264954</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F3" t="s">
         <v>72</v>
       </c>
       <c r="G3" t="s">
-        <v>78</v>
+        <v>84</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1177,7 +1363,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1301,7 +1487,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E7" t="s">
         <v>59</v>
@@ -1335,7 +1521,7 @@
         <v>7</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E9" t="s">
         <v>61</v>
@@ -1352,7 +1538,7 @@
         <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E10" t="s">
         <v>65</v>
@@ -1364,6 +1550,98 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15D1676A-B11A-4778-BA33-295949D1EBED}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="54" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>14509287</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>10009287</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECF3BD9F-BB2C-4762-9B75-35EAD51DD955}">
   <dimension ref="A1:AD2"/>
   <sheetViews>
@@ -1536,7 +1814,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62512D92-1B60-4099-B0C3-A81E1B8F00EF}">
   <dimension ref="A1:E13"/>
   <sheetViews>
@@ -1778,7 +2056,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B94867E-CC6C-41F2-AD37-D0702267E417}">
   <dimension ref="A1:F17"/>
   <sheetViews>
@@ -2140,167 +2418,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A722FA9C-9A5F-4297-AFA4-6881D5BABD53}">
-  <dimension ref="A1:F7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="46.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1039458363</v>
-      </c>
-      <c r="E5" t="s">
-        <v>69</v>
-      </c>
-      <c r="F5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="1">
-        <v>1039458363</v>
-      </c>
-      <c r="E6" t="s">
-        <v>69</v>
-      </c>
-      <c r="F6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>